<commit_message>
fix(template), #516: Add missing model scores in output file.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C20D0D-4B02-EF4B-93C9-4855479BA645}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="37395" windowHeight="16755"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="4" r:id="rId1"/>
     <sheet name="dice_report" sheetId="5" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="81">
   <si>
     <t>Vehicle Family ID</t>
   </si>
@@ -437,11 +450,23 @@
   <si>
     <t>Model_scores WLTP-L</t>
   </si>
+  <si>
+    <t>electrics_model (service battery currents)</t>
+  </si>
+  <si>
+    <t>electrics_model (alternator currents)</t>
+  </si>
+  <si>
+    <t>electrics_model (drive battery currents)</t>
+  </si>
+  <si>
+    <t>electrics_model (dc/dc converter currents)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -812,32 +837,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -960,6 +959,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1015,10 +1042,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -1075,14 +1098,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="5" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection hidden="1"/>
@@ -1199,6 +1214,14 @@
       <alignment horizontal="center" vertical="top"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
@@ -1207,7 +1230,11 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1215,15 +1242,31 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1231,62 +1274,46 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1315,6 +1342,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1363,7 +1393,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1396,9 +1426,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1431,6 +1478,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1606,32 +1670,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="1.1640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="3" customWidth="1"/>
     <col min="4" max="5" width="12" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="1.140625" style="54" customWidth="1"/>
-    <col min="9" max="9" width="1.140625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" style="3" customWidth="1"/>
-    <col min="12" max="15" width="12" style="3" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="1.140625" style="10" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="3" hidden="1"/>
+    <col min="6" max="6" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.1640625" style="51" customWidth="1"/>
+    <col min="8" max="8" width="1.1640625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="3" customWidth="1"/>
+    <col min="11" max="14" width="10.6640625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.83203125" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="15.75" customHeight="1">
+    <row r="1" spans="2:19" ht="15.75" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1641,27 +1703,25 @@
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="2" t="str">
+      <c r="J1" s="2" t="str">
         <f ca="1">C1</f>
         <v/>
       </c>
+      <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
-      <c r="Q1" s="5"/>
+      <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-    </row>
-    <row r="2" spans="2:21" ht="15.75" customHeight="1">
+    </row>
+    <row r="2" spans="2:19" ht="15.75" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1671,27 +1731,25 @@
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="2" t="str">
+      <c r="J2" s="2" t="str">
         <f ca="1">C2</f>
         <v/>
       </c>
+      <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
-      <c r="Q2" s="7"/>
+      <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-    </row>
-    <row r="3" spans="2:21" ht="15.75" customHeight="1">
+    </row>
+    <row r="3" spans="2:19" ht="15.75" customHeight="1">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1701,27 +1759,25 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="2" t="str">
+      <c r="J3" s="2" t="str">
         <f ca="1">C3</f>
         <v/>
       </c>
+      <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
-      <c r="Q3" s="7"/>
+      <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-    </row>
-    <row r="4" spans="2:21" ht="15.75" customHeight="1">
+    </row>
+    <row r="4" spans="2:19" ht="15.75" customHeight="1">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1731,1152 +1787,1142 @@
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="J4" s="1" t="s">
+      <c r="G4" s="10"/>
+      <c r="I4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="8" t="str">
+      <c r="J4" s="8" t="str">
         <f ca="1">C4</f>
         <v/>
       </c>
+      <c r="L4" s="9"/>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
       <c r="R4" s="9"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-    </row>
-    <row r="5" spans="2:21" ht="15.75" customHeight="1">
+    </row>
+    <row r="5" spans="2:19" ht="15.75" customHeight="1">
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-    </row>
-    <row r="6" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
+    </row>
+    <row r="6" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="11" t="s">
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="68"/>
-      <c r="Q6" s="13"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-    </row>
-    <row r="7" spans="2:21" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
+    </row>
+    <row r="7" spans="2:19" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="G7" s="10"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-    </row>
-    <row r="8" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B8" s="63" t="s">
+    </row>
+    <row r="8" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B8" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="14" t="s">
+      <c r="C8" s="61"/>
+      <c r="D8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="10"/>
-      <c r="L8" s="79" t="s">
+      <c r="G8" s="10"/>
+      <c r="K8" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="78"/>
-      <c r="N8" s="79" t="s">
+      <c r="L8" s="75"/>
+      <c r="M8" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="78"/>
+      <c r="N8" s="75"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-    </row>
-    <row r="9" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B9" s="59" t="s">
+    </row>
+    <row r="9" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B9" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="17" t="str">
+      <c r="C9" s="57"/>
+      <c r="D9" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_target_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="E9" s="18" t="str">
+      <c r="E9" s="17" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_target_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="10"/>
-      <c r="J9" s="71" t="s">
+      <c r="G9" s="10"/>
+      <c r="I9" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="72"/>
-      <c r="L9" s="20" t="s">
+      <c r="J9" s="69"/>
+      <c r="K9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="L9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="20" t="s">
+      <c r="M9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="O9" s="15" t="s">
+      <c r="N9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="77" t="s">
+      <c r="O9" s="74" t="s">
         <v>7</v>
       </c>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-    </row>
-    <row r="10" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B10" s="61" t="s">
+    </row>
+    <row r="10" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B10" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="21" t="str">
+      <c r="C10" s="59"/>
+      <c r="D10" s="20" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="E10" s="22" t="str">
+      <c r="E10" s="21" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="J10" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="73"/>
+      <c r="G10" s="10"/>
+      <c r="I10" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="70"/>
+      <c r="K10" s="22" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_service_battery_currents_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
       <c r="L10" s="23" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_battery_currents_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M10" s="24" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_battery_currents_wltp_h_wltp_l_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_service_battery_currents_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M10" s="22" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_service_battery_currents_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
       <c r="N10" s="23" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_battery_currents_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O10" s="24" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_battery_currents_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="P10" s="25" t="s">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_service_battery_currents_wltp_l_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O10" s="24" t="s">
         <v>13</v>
       </c>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-    </row>
-    <row r="11" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B11" s="65" t="s">
+    </row>
+    <row r="11" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B11" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="26" t="str">
+      <c r="C11" s="63"/>
+      <c r="D11" s="25" t="str">
         <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100,"")</f>
         <v/>
       </c>
-      <c r="E11" s="27" t="str">
+      <c r="E11" s="26" t="str">
         <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio")-1)*100, "")</f>
         <v/>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
-      <c r="J11" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="74"/>
-      <c r="L11" s="28" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_alternator_currents_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M11" s="29" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_alternator_currents_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N11" s="28" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_alternator_currents_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O11" s="29" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_alternator_currents_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="P11" s="25" t="s">
+      <c r="G11" s="10"/>
+      <c r="I11" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="79"/>
+      <c r="K11" s="80" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_alternator_currents_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="L11" s="81" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_alternator_currents_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M11" s="80" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_alternator_currents_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N11" s="81" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_alternator_currents_wltp_l_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O11" s="24" t="s">
         <v>13</v>
       </c>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-    </row>
-    <row r="12" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B12" s="67" t="s">
+    </row>
+    <row r="12" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B12" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="J12" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="76"/>
-      <c r="L12" s="31" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M12" s="32" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N12" s="31" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O12" s="32" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="P12" s="19" t="s">
-        <v>18</v>
-      </c>
+      <c r="G12" s="10"/>
+      <c r="I12" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" s="79"/>
+      <c r="K12" s="80" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_drive_battery_currents_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="L12" s="81" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_drive_battery_currents_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M12" s="80" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_drive_battery_currents_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N12" s="81" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_drive_battery_currents_wltp_l_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O12" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
       <c r="R12" s="9"/>
       <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-    </row>
-    <row r="13" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
+    </row>
+    <row r="13" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
       <c r="C13" s="4"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="J13" s="75" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="76"/>
-      <c r="L13" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M13" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N13" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O13" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="P13" s="19" t="s">
-        <v>20</v>
-      </c>
+      <c r="G13" s="10"/>
+      <c r="I13" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="71"/>
+      <c r="K13" s="37" t="str">
+        <f ca="1">IF(K12&lt;&gt;"",IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_dcdc_converter_currents_wltp_h_wltp_h_score"),""),"")</f>
+        <v/>
+      </c>
+      <c r="L13" s="38" t="str">
+        <f ca="1">IF(K12&lt;&gt;"",IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_dcdc_converter_currents_wltp_h_wltp_l_score"),""),"")</f>
+        <v/>
+      </c>
+      <c r="M13" s="37" t="str">
+        <f ca="1">IF(K12&lt;&gt;"",IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_dcdc_converter_currents_wltp_l_wltp_h_score"),""),"")</f>
+        <v/>
+      </c>
+      <c r="N13" s="38" t="str">
+        <f ca="1">IF(K12&lt;&gt;"",IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_dcdc_converter_currents_wltp_l_wltp_l_score"),""),"")</f>
+        <v/>
+      </c>
+      <c r="O13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
       <c r="R13" s="9"/>
       <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-    </row>
-    <row r="14" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B14" s="63" t="s">
+    </row>
+    <row r="14" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B14" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="64"/>
-      <c r="D14" s="14" t="s">
+      <c r="C14" s="61"/>
+      <c r="D14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="10"/>
-      <c r="J14" s="75" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="76"/>
-      <c r="L14" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M14" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N14" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O14" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="P14" s="19" t="s">
-        <v>22</v>
-      </c>
+      <c r="G14" s="10"/>
+      <c r="I14" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="73"/>
+      <c r="K14" s="28" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="L14" s="29" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M14" s="28" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N14" s="29" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_l_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
       <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-    </row>
-    <row r="15" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B15" s="59" t="s">
+    </row>
+    <row r="15" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B15" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="60"/>
-      <c r="D15" s="34" t="str">
+      <c r="C15" s="57"/>
+      <c r="D15" s="31" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="E15" s="35" t="str">
+      <c r="E15" s="32" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_value__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
-      <c r="J15" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="76"/>
-      <c r="L15" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M15" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N15" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O15" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="P15" s="19" t="s">
+      <c r="G15" s="10"/>
+      <c r="I15" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="73"/>
+      <c r="K15" s="28" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="L15" s="29" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M15" s="28" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N15" s="29" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O15" s="18" t="s">
         <v>20</v>
       </c>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-    </row>
-    <row r="16" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B16" s="61" t="s">
+    </row>
+    <row r="16" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B16" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="21" t="str">
+      <c r="C16" s="59"/>
+      <c r="D16" s="20" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="E16" s="22" t="str">
+      <c r="E16" s="21" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_UDC__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="10"/>
-      <c r="J16" s="75" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="76"/>
-      <c r="L16" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M16" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N16" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O16" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="P16" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="G16" s="10"/>
+      <c r="I16" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="73"/>
+      <c r="K16" s="28" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="L16" s="29" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M16" s="28" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N16" s="29" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_l_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O16" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
-    </row>
-    <row r="17" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B17" s="65" t="s">
+    </row>
+    <row r="17" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B17" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="36" t="str">
+      <c r="C17" s="63"/>
+      <c r="D17" s="33" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="E17" s="37" t="str">
+      <c r="E17" s="34" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_EUDC__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="10"/>
-      <c r="J17" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="K17" s="76"/>
-      <c r="L17" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M17" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N17" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O17" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="P17" s="19" t="s">
+      <c r="G17" s="10"/>
+      <c r="I17" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="73"/>
+      <c r="K17" s="28" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="L17" s="29" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M17" s="28" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N17" s="29" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O17" s="18" t="s">
         <v>20</v>
       </c>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-    </row>
-    <row r="18" spans="2:21" ht="15.75" customHeight="1">
-      <c r="C18" s="38"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
+    </row>
+    <row r="18" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="10"/>
-      <c r="J18" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="K18" s="73"/>
-      <c r="L18" s="23" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M18" s="24" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N18" s="23" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O18" s="24" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="P18" s="19" t="s">
-        <v>18</v>
-      </c>
+      <c r="G18" s="10"/>
+      <c r="I18" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="73"/>
+      <c r="K18" s="28" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="L18" s="29" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M18" s="28" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N18" s="29" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_l_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O18" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
-    </row>
-    <row r="19" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B19" s="68"/>
-      <c r="C19" s="68"/>
+    </row>
+    <row r="19" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
       <c r="D19" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="K19" s="74"/>
-      <c r="L19" s="40" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M19" s="41" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N19" s="40" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O19" s="41" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="P19" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q19" s="7"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="73"/>
+      <c r="K19" s="28" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="L19" s="29" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M19" s="28" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N19" s="29" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O19" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-    </row>
-    <row r="20" spans="2:21" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="G20" s="9"/>
-      <c r="H20" s="10"/>
-      <c r="J20" s="9"/>
+    </row>
+    <row r="20" spans="2:19" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="G20" s="10"/>
+      <c r="I20" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="70"/>
+      <c r="K20" s="22" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="L20" s="23" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M20" s="22" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N20" s="23" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O20" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-    </row>
-    <row r="21" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B21" s="63" t="s">
+    </row>
+    <row r="21" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B21" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="64"/>
-      <c r="D21" s="14" t="s">
+      <c r="C21" s="61"/>
+      <c r="D21" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
-      <c r="J21" s="9"/>
+      <c r="G21" s="10"/>
+      <c r="I21" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="71"/>
+      <c r="K21" s="37" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="L21" s="38" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M21" s="37" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N21" s="38" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O21" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-    </row>
-    <row r="22" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B22" s="59" t="s">
+    </row>
+    <row r="22" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B22" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="34" t="str">
+      <c r="C22" s="57"/>
+      <c r="D22" s="31" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__"),"")</f>
         <v/>
       </c>
-      <c r="E22" s="35" t="str">
+      <c r="E22" s="32" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_fuel_type__"),"")</f>
         <v/>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="F22" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="10"/>
-      <c r="J22" s="9"/>
+      <c r="G22" s="10"/>
+      <c r="I22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-    </row>
-    <row r="23" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B23" s="61" t="s">
+    </row>
+    <row r="23" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B23" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="42" t="str">
+      <c r="C23" s="59"/>
+      <c r="D23" s="39" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
         <v/>
       </c>
-      <c r="E23" s="43" t="str">
+      <c r="E23" s="40" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
         <v/>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="10"/>
-      <c r="J23" s="9"/>
+      <c r="G23" s="10"/>
+      <c r="I23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-    </row>
-    <row r="24" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B24" s="61" t="s">
+    </row>
+    <row r="24" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B24" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="42" t="str">
+      <c r="C24" s="59"/>
+      <c r="D24" s="39" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),"")</f>
         <v/>
       </c>
-      <c r="E24" s="43" t="str">
+      <c r="E24" s="40" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__"),"")</f>
         <v/>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="10"/>
-      <c r="J24" s="9"/>
+      <c r="G24" s="10"/>
+      <c r="I24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-    </row>
-    <row r="25" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B25" s="65" t="s">
+    </row>
+    <row r="25" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B25" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="66"/>
-      <c r="D25" s="44" t="str">
+      <c r="C25" s="63"/>
+      <c r="D25" s="41" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),"")</f>
         <v/>
       </c>
-      <c r="E25" s="45" t="str">
+      <c r="E25" s="42" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__"),"")</f>
         <v/>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="10"/>
-      <c r="J25" s="9"/>
+      <c r="G25" s="10"/>
+      <c r="I25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-    </row>
-    <row r="26" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="C26" s="38"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
+    </row>
+    <row r="26" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="C26" s="35"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="10"/>
-      <c r="J26" s="9"/>
+      <c r="G26" s="10"/>
+      <c r="I26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-    </row>
-    <row r="27" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B27" s="63" t="s">
+    </row>
+    <row r="27" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B27" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="64"/>
-      <c r="D27" s="14" t="s">
+      <c r="C27" s="61"/>
+      <c r="D27" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10"/>
-      <c r="J27" s="9"/>
+      <c r="G27" s="10"/>
+      <c r="I27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="9"/>
-    </row>
-    <row r="28" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B28" s="59" t="s">
+    </row>
+    <row r="28" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B28" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="21" t="str">
+      <c r="C28" s="57"/>
+      <c r="D28" s="20" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_"),"")</f>
         <v/>
       </c>
-      <c r="E28" s="22" t="str">
+      <c r="E28" s="21" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f0__N_"),"")</f>
         <v/>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
-      <c r="U28" s="9"/>
-    </row>
-    <row r="29" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B29" s="69" t="s">
+    </row>
+    <row r="29" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B29" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="70"/>
-      <c r="D29" s="47" t="str">
+      <c r="C29" s="67"/>
+      <c r="D29" s="44" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
-      <c r="E29" s="48" t="str">
+      <c r="E29" s="45" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-    </row>
-    <row r="30" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B30" s="69" t="s">
+    </row>
+    <row r="30" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B30" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="70"/>
-      <c r="D30" s="47" t="str">
+      <c r="C30" s="67"/>
+      <c r="D30" s="44" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
-      <c r="E30" s="48" t="str">
+      <c r="E30" s="45" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-    </row>
-    <row r="31" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="65" t="s">
+    </row>
+    <row r="31" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B31" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="66"/>
-      <c r="D31" s="49" t="str">
+      <c r="C31" s="63"/>
+      <c r="D31" s="46" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_"),"")</f>
         <v/>
       </c>
-      <c r="E31" s="50" t="str">
+      <c r="E31" s="47" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_mass__kg_"),"")</f>
         <v/>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
-    </row>
-    <row r="32" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
+    </row>
+    <row r="32" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
       <c r="F32" s="10"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-    </row>
-    <row r="33" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B33" s="63" t="s">
+    </row>
+    <row r="33" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B33" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="64"/>
-      <c r="D33" s="14" t="s">
+      <c r="C33" s="61"/>
+      <c r="D33" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G33" s="9"/>
-      <c r="H33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="U33" s="9"/>
-    </row>
-    <row r="34" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B34" s="59" t="s">
+    </row>
+    <row r="34" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B34" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="60"/>
-      <c r="D34" s="21" t="str">
+      <c r="C34" s="57"/>
+      <c r="D34" s="20" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_"),"")</f>
         <v/>
       </c>
-      <c r="E34" s="22" t="str">
+      <c r="E34" s="21" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f0__N_"),"")</f>
         <v/>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F34" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
       <c r="R34" s="9"/>
       <c r="S34" s="9"/>
-      <c r="T34" s="9"/>
-      <c r="U34" s="9"/>
-    </row>
-    <row r="35" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B35" s="69" t="s">
+    </row>
+    <row r="35" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B35" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="70"/>
-      <c r="D35" s="47" t="str">
+      <c r="C35" s="67"/>
+      <c r="D35" s="44" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
-      <c r="E35" s="48" t="str">
+      <c r="E35" s="45" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
-      <c r="F35" s="19" t="s">
+      <c r="F35" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G35" s="9"/>
-      <c r="H35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
       <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-    </row>
-    <row r="36" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B36" s="69" t="s">
+    </row>
+    <row r="36" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B36" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="70"/>
-      <c r="D36" s="47" t="str">
+      <c r="C36" s="67"/>
+      <c r="D36" s="44" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
-      <c r="E36" s="48" t="str">
+      <c r="E36" s="45" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G36" s="9"/>
-      <c r="H36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
       <c r="S36" s="9"/>
-      <c r="T36" s="9"/>
-      <c r="U36" s="9"/>
-    </row>
-    <row r="37" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B37" s="61" t="s">
+    </row>
+    <row r="37" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B37" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="62"/>
-      <c r="D37" s="52" t="str">
+      <c r="C37" s="59"/>
+      <c r="D37" s="49" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_"),"")</f>
         <v/>
       </c>
-      <c r="E37" s="53" t="str">
+      <c r="E37" s="50" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_mass__kg_"),"")</f>
         <v/>
       </c>
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G37" s="9"/>
-      <c r="H37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
       <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
-      <c r="U37" s="9"/>
-    </row>
-    <row r="38" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B38" s="61" t="s">
+    </row>
+    <row r="38" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B38" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="62"/>
-      <c r="D38" s="21" t="str">
+      <c r="C38" s="59"/>
+      <c r="D38" s="20" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="E38" s="22" t="str">
+      <c r="E38" s="21" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
       <c r="S38" s="9"/>
-      <c r="T38" s="9"/>
-      <c r="U38" s="9"/>
-    </row>
-    <row r="39" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B39" s="61" t="s">
+    </row>
+    <row r="39" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B39" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="62"/>
-      <c r="D39" s="21" t="str">
+      <c r="C39" s="59"/>
+      <c r="D39" s="20" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="E39" s="22" t="str">
+      <c r="E39" s="21" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="F39" s="19" t="s">
+      <c r="F39" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="9"/>
-      <c r="H39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
       <c r="S39" s="9"/>
-      <c r="T39" s="9"/>
-      <c r="U39" s="9"/>
-    </row>
-    <row r="40" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B40" s="61" t="s">
+    </row>
+    <row r="40" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B40" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="62"/>
-      <c r="D40" s="21" t="str">
+      <c r="C40" s="59"/>
+      <c r="D40" s="20" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="E40" s="22" t="str">
+      <c r="E40" s="21" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="F40" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
       <c r="S40" s="9"/>
-      <c r="T40" s="9"/>
-      <c r="U40" s="9"/>
-    </row>
-    <row r="41" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B41" s="65" t="s">
+    </row>
+    <row r="41" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B41" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="C41" s="66"/>
-      <c r="D41" s="36" t="str">
+      <c r="C41" s="63"/>
+      <c r="D41" s="33" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="E41" s="37" t="str">
+      <c r="E41" s="34" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="F41" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="9"/>
-      <c r="H41" s="10"/>
-      <c r="J41" s="9"/>
+      <c r="G41" s="10"/>
+      <c r="I41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
       <c r="S41" s="9"/>
-      <c r="T41" s="9"/>
-      <c r="U41" s="9"/>
-    </row>
-    <row r="42" spans="2:21" ht="15.75" customHeight="1">
-      <c r="G42" s="9"/>
-      <c r="H42" s="10"/>
-      <c r="J42" s="9"/>
+    </row>
+    <row r="42" spans="2:19" ht="15.75" customHeight="1">
+      <c r="G42" s="10"/>
+      <c r="I42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="9"/>
       <c r="S42" s="9"/>
-      <c r="T42" s="9"/>
-      <c r="U42" s="9"/>
-    </row>
-    <row r="43" spans="2:21" ht="15.75" customHeight="1">
-      <c r="G43" s="9"/>
-      <c r="H43" s="10"/>
-      <c r="J43" s="9"/>
+    </row>
+    <row r="43" spans="2:19" ht="15.75" customHeight="1">
+      <c r="G43" s="10"/>
+      <c r="I43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="9"/>
       <c r="S43" s="9"/>
-      <c r="T43" s="9"/>
-      <c r="U43" s="9"/>
-    </row>
-    <row r="44" spans="2:21" ht="15.75" customHeight="1">
-      <c r="G44" s="9"/>
-      <c r="H44" s="10"/>
-      <c r="J44" s="9"/>
+    </row>
+    <row r="44" spans="2:19" ht="15.75" customHeight="1">
+      <c r="G44" s="10"/>
+      <c r="I44" s="9"/>
+      <c r="Q44" s="9"/>
+      <c r="R44" s="9"/>
       <c r="S44" s="9"/>
-      <c r="T44" s="9"/>
-      <c r="U44" s="9"/>
-    </row>
-    <row r="45" spans="2:21" ht="15.75" customHeight="1">
-      <c r="G45" s="9"/>
-      <c r="H45" s="10"/>
-      <c r="J45" s="9"/>
+    </row>
+    <row r="45" spans="2:19" ht="15.75" customHeight="1">
+      <c r="G45" s="10"/>
+      <c r="I45" s="9"/>
+      <c r="Q45" s="9"/>
+      <c r="R45" s="9"/>
       <c r="S45" s="9"/>
-      <c r="T45" s="9"/>
-      <c r="U45" s="9"/>
-    </row>
-    <row r="46" spans="2:21" ht="15.75" customHeight="1">
-      <c r="G46" s="9"/>
-      <c r="H46" s="10"/>
-      <c r="J46" s="9"/>
+    </row>
+    <row r="46" spans="2:19" ht="15.75" customHeight="1">
+      <c r="G46" s="10"/>
+      <c r="I46" s="9"/>
+      <c r="Q46" s="9"/>
+      <c r="R46" s="9"/>
       <c r="S46" s="9"/>
-      <c r="T46" s="9"/>
-      <c r="U46" s="9"/>
-    </row>
-    <row r="47" spans="2:21" ht="15.75" customHeight="1">
-      <c r="G47" s="9"/>
-      <c r="H47" s="10"/>
-      <c r="J47" s="9"/>
+    </row>
+    <row r="47" spans="2:19" ht="15.75" customHeight="1">
+      <c r="G47" s="10"/>
+      <c r="I47" s="9"/>
+      <c r="Q47" s="9"/>
+      <c r="R47" s="9"/>
       <c r="S47" s="9"/>
-      <c r="T47" s="9"/>
-      <c r="U47" s="9"/>
-    </row>
-    <row r="48" spans="2:21" ht="15.75" hidden="1" customHeight="1">
-      <c r="G48" s="9"/>
-      <c r="H48" s="10"/>
-      <c r="J48" s="9"/>
+    </row>
+    <row r="48" spans="2:19" ht="15.75" hidden="1" customHeight="1">
+      <c r="G48" s="10"/>
+      <c r="I48" s="9"/>
+      <c r="Q48" s="9"/>
+      <c r="R48" s="9"/>
       <c r="S48" s="9"/>
-      <c r="T48" s="9"/>
-      <c r="U48" s="9"/>
-    </row>
-    <row r="49" spans="3:21" ht="15.75" hidden="1" customHeight="1">
-      <c r="G49" s="9"/>
-      <c r="H49" s="10"/>
-      <c r="J49" s="9"/>
+    </row>
+    <row r="49" spans="3:19" ht="15.75" hidden="1" customHeight="1">
+      <c r="G49" s="10"/>
+      <c r="I49" s="9"/>
+      <c r="P49" s="9"/>
+      <c r="Q49" s="9"/>
       <c r="R49" s="9"/>
       <c r="S49" s="9"/>
-      <c r="T49" s="9"/>
-      <c r="U49" s="9"/>
-    </row>
-    <row r="50" spans="3:21" ht="15" hidden="1" customHeight="1">
+    </row>
+    <row r="50" spans="3:19" ht="15" hidden="1" customHeight="1">
       <c r="C50" s="6"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
+      <c r="G50" s="5"/>
       <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="4"/>
-      <c r="Q50" s="5"/>
+      <c r="I50" s="4"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
       <c r="R50" s="9"/>
       <c r="S50" s="9"/>
-      <c r="T50" s="9"/>
-      <c r="U50" s="9"/>
-    </row>
-    <row r="51" spans="3:21" ht="15" hidden="1" customHeight="1">
+    </row>
+    <row r="51" spans="3:19" ht="15" hidden="1" customHeight="1">
       <c r="C51" s="6"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
+      <c r="G51" s="5"/>
       <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="4"/>
-      <c r="Q51" s="5"/>
+      <c r="I51" s="4"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="9"/>
       <c r="R51" s="9"/>
       <c r="S51" s="9"/>
-      <c r="T51" s="9"/>
-      <c r="U51" s="9"/>
-    </row>
-    <row r="52" spans="3:21" ht="15" hidden="1" customHeight="1">
+    </row>
+    <row r="52" spans="3:19" ht="15" hidden="1" customHeight="1">
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+      <c r="G52" s="7"/>
       <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
+      <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
       <c r="N52" s="6"/>
-      <c r="O52" s="6"/>
+      <c r="O52" s="9"/>
       <c r="P52" s="9"/>
-      <c r="Q52" s="7"/>
+      <c r="Q52" s="9"/>
       <c r="R52" s="9"/>
       <c r="S52" s="9"/>
-      <c r="T52" s="9"/>
-      <c r="U52" s="9"/>
-    </row>
-    <row r="53" spans="3:21" ht="15" hidden="1" customHeight="1">
+    </row>
+    <row r="53" spans="3:19" ht="15" hidden="1" customHeight="1">
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
@@ -2884,18 +2930,17 @@
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
       <c r="P53" s="9"/>
+      <c r="Q53" s="9"/>
       <c r="R53" s="9"/>
       <c r="S53" s="9"/>
-      <c r="T53" s="9"/>
-      <c r="U53" s="9"/>
-    </row>
-    <row r="54" spans="3:21" ht="15" hidden="1" customHeight="1">
+    </row>
+    <row r="54" spans="3:19" ht="15" hidden="1" customHeight="1">
       <c r="C54" s="6"/>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="I54" s="9"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
@@ -2903,18 +2948,17 @@
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
       <c r="P54" s="9"/>
+      <c r="Q54" s="9"/>
       <c r="R54" s="9"/>
       <c r="S54" s="9"/>
-      <c r="T54" s="9"/>
-      <c r="U54" s="9"/>
-    </row>
-    <row r="55" spans="3:21" ht="15" hidden="1" customHeight="1">
+    </row>
+    <row r="55" spans="3:19" ht="15" hidden="1" customHeight="1">
       <c r="C55" s="6"/>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="I55" s="9"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
@@ -2922,18 +2966,17 @@
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
       <c r="P55" s="9"/>
+      <c r="Q55" s="9"/>
       <c r="R55" s="9"/>
       <c r="S55" s="9"/>
-      <c r="T55" s="9"/>
-      <c r="U55" s="9"/>
-    </row>
-    <row r="56" spans="3:21" ht="15" hidden="1" customHeight="1">
+    </row>
+    <row r="56" spans="3:19" ht="15" hidden="1" customHeight="1">
       <c r="C56" s="6"/>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="I56" s="9"/>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
       <c r="L56" s="9"/>
@@ -2941,18 +2984,17 @@
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
       <c r="P56" s="9"/>
+      <c r="Q56" s="9"/>
       <c r="R56" s="9"/>
       <c r="S56" s="9"/>
-      <c r="T56" s="9"/>
-      <c r="U56" s="9"/>
-    </row>
-    <row r="57" spans="3:21" ht="15" hidden="1" customHeight="1">
+    </row>
+    <row r="57" spans="3:19" ht="15" hidden="1" customHeight="1">
       <c r="C57" s="6"/>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
@@ -2960,18 +3002,17 @@
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
       <c r="P57" s="9"/>
+      <c r="Q57" s="9"/>
       <c r="R57" s="9"/>
       <c r="S57" s="9"/>
-      <c r="T57" s="9"/>
-      <c r="U57" s="9"/>
-    </row>
-    <row r="58" spans="3:21" ht="15" hidden="1" customHeight="1">
+    </row>
+    <row r="58" spans="3:19" ht="15" hidden="1" customHeight="1">
       <c r="C58" s="6"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
@@ -2979,18 +3020,17 @@
       <c r="N58" s="9"/>
       <c r="O58" s="9"/>
       <c r="P58" s="9"/>
+      <c r="Q58" s="9"/>
       <c r="R58" s="9"/>
       <c r="S58" s="9"/>
-      <c r="T58" s="9"/>
-      <c r="U58" s="9"/>
-    </row>
-    <row r="59" spans="3:21" ht="15" hidden="1" customHeight="1">
+    </row>
+    <row r="59" spans="3:19" ht="15" hidden="1" customHeight="1">
       <c r="C59" s="6"/>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
@@ -2998,18 +3038,17 @@
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
       <c r="P59" s="9"/>
+      <c r="Q59" s="9"/>
       <c r="R59" s="9"/>
       <c r="S59" s="9"/>
-      <c r="T59" s="9"/>
-      <c r="U59" s="9"/>
-    </row>
-    <row r="60" spans="3:21" ht="15" hidden="1" customHeight="1">
+    </row>
+    <row r="60" spans="3:19" ht="15" hidden="1" customHeight="1">
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="I60" s="9"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
@@ -3017,15 +3056,14 @@
       <c r="N60" s="9"/>
       <c r="O60" s="9"/>
       <c r="P60" s="9"/>
+      <c r="Q60" s="9"/>
       <c r="R60" s="9"/>
       <c r="S60" s="9"/>
-      <c r="T60" s="9"/>
-      <c r="U60" s="9"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="D11:E11">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="num" val="-4"/>
         <cfvo type="num" val="0"/>
@@ -3036,8 +3074,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L12">
-    <cfRule type="colorScale" priority="38">
+  <conditionalFormatting sqref="K14">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -3046,8 +3084,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M13">
-    <cfRule type="colorScale" priority="40">
+  <conditionalFormatting sqref="L15">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3056,8 +3094,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10">
-    <cfRule type="colorScale" priority="25">
+  <conditionalFormatting sqref="N10">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3066,8 +3104,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L11">
-    <cfRule type="colorScale" priority="39">
+  <conditionalFormatting sqref="K11">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3076,8 +3114,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
-    <cfRule type="colorScale" priority="37">
+  <conditionalFormatting sqref="K15">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3086,8 +3124,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L14">
-    <cfRule type="colorScale" priority="36">
+  <conditionalFormatting sqref="K16">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3096,8 +3134,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L15">
-    <cfRule type="colorScale" priority="35">
+  <conditionalFormatting sqref="K17">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3106,8 +3144,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L16">
-    <cfRule type="colorScale" priority="34">
+  <conditionalFormatting sqref="K18">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -3116,8 +3154,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L17">
-    <cfRule type="colorScale" priority="33">
+  <conditionalFormatting sqref="K19">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -3126,8 +3164,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19">
-    <cfRule type="colorScale" priority="32">
+  <conditionalFormatting sqref="K21">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3136,8 +3174,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L10">
-    <cfRule type="colorScale" priority="31">
+  <conditionalFormatting sqref="K10">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3146,8 +3184,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O12">
-    <cfRule type="colorScale" priority="22">
+  <conditionalFormatting sqref="N14">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -3156,8 +3194,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11">
-    <cfRule type="colorScale" priority="30">
+  <conditionalFormatting sqref="L11">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3166,8 +3204,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M10">
-    <cfRule type="colorScale" priority="29">
+  <conditionalFormatting sqref="L10">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3176,8 +3214,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N11">
-    <cfRule type="colorScale" priority="28">
+  <conditionalFormatting sqref="M11">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3186,8 +3224,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N10">
-    <cfRule type="colorScale" priority="27">
+  <conditionalFormatting sqref="M10">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3196,8 +3234,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O11">
-    <cfRule type="colorScale" priority="26">
+  <conditionalFormatting sqref="N11">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3206,8 +3244,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M12">
-    <cfRule type="colorScale" priority="24">
+  <conditionalFormatting sqref="L14">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -3216,8 +3254,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N12">
-    <cfRule type="colorScale" priority="23">
+  <conditionalFormatting sqref="M14">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -3226,8 +3264,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O13">
-    <cfRule type="colorScale" priority="21">
+  <conditionalFormatting sqref="N15">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3236,8 +3274,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N13">
-    <cfRule type="colorScale" priority="20">
+  <conditionalFormatting sqref="M15">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3246,8 +3284,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14">
-    <cfRule type="colorScale" priority="19">
+  <conditionalFormatting sqref="L16">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3256,8 +3294,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N14">
-    <cfRule type="colorScale" priority="18">
+  <conditionalFormatting sqref="M16">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3266,8 +3304,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O14">
-    <cfRule type="colorScale" priority="17">
+  <conditionalFormatting sqref="N16">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3276,8 +3314,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M15">
-    <cfRule type="colorScale" priority="16">
+  <conditionalFormatting sqref="L17">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3286,8 +3324,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N15">
-    <cfRule type="colorScale" priority="15">
+  <conditionalFormatting sqref="M17">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3296,8 +3334,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O15">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="N17">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3306,8 +3344,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M16">
-    <cfRule type="colorScale" priority="13">
+  <conditionalFormatting sqref="L18">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -3316,8 +3354,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N16">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="M18">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -3326,8 +3364,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O16">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="N18">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -3336,8 +3374,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M17">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="L19">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -3346,8 +3384,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N17">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="M19">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -3356,8 +3394,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O17">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="N19">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -3366,8 +3404,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L18">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="K20">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3376,8 +3414,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M18">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="L20">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3386,8 +3424,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N18">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="M20">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3396,8 +3434,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="N20">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3406,8 +3444,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M19">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="L21">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3416,8 +3454,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N19">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="M21">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3426,8 +3464,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O19">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="N21">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3436,12 +3474,92 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4 K4">
-    <cfRule type="expression" dxfId="1" priority="42">
+  <conditionalFormatting sqref="C4 J4">
+    <cfRule type="expression" dxfId="1" priority="50">
       <formula>$C$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="43">
+    <cfRule type="expression" dxfId="0" priority="51">
       <formula>$C$4="True"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N12">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L12">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M12">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N13">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L13">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M13">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3450,32 +3568,35 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Bold"CO&amp;Y2&amp;YMPAS SUMMARY OUTPUT REPORT</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="6" max="1048575" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.5703125" style="58" customWidth="1"/>
-    <col min="4" max="4" width="8" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" style="58" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.85546875" style="58"/>
+    <col min="1" max="1" width="34.5" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.5" style="55" customWidth="1"/>
+    <col min="4" max="4" width="8" style="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" style="55" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.83203125" style="55"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="52" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3544,347 +3665,347 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="56" t="str">
+      <c r="B7" s="53" t="str">
         <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100,"")</f>
         <v/>
       </c>
-      <c r="C7" s="56" t="str">
+      <c r="C7" s="53" t="str">
         <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio")-1)*100,"")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
     </row>
     <row r="9" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="42" t="str">
+      <c r="B9" s="39" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__"),"")</f>
         <v/>
       </c>
-      <c r="C9" s="42" t="str">
+      <c r="C9" s="39" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_fuel_type__"),"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="42" t="str">
+      <c r="B10" s="39" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
         <v/>
       </c>
-      <c r="C10" s="42" t="str">
+      <c r="C10" s="39" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="42" t="str">
+      <c r="B11" s="39" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),"")</f>
         <v/>
       </c>
-      <c r="C11" s="42" t="str">
+      <c r="C11" s="39" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__"),"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="42" t="str">
+      <c r="B12" s="39" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),"")</f>
         <v/>
       </c>
-      <c r="C12" s="42" t="str">
+      <c r="C12" s="39" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__"),"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
     </row>
     <row r="14" spans="1:3" ht="15">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="81" t="str">
+      <c r="B14" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_battery_currents_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C14" s="81" t="str">
+      <c r="C14" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_battery_currents_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="81" t="str">
+      <c r="B15" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_alternator_currents_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C15" s="81" t="str">
+      <c r="C15" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_alternator_currents_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="81" t="str">
+      <c r="B16" s="78" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C16" s="81" t="str">
+      <c r="C16" s="78" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15">
-      <c r="A17" s="80" t="s">
+      <c r="A17" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="81" t="str">
+      <c r="B17" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C17" s="81" t="str">
+      <c r="C17" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15">
-      <c r="A18" s="80" t="s">
+      <c r="A18" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="81" t="str">
+      <c r="B18" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C18" s="81" t="str">
+      <c r="C18" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="81" t="str">
+      <c r="B19" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C19" s="81" t="str">
+      <c r="C19" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15">
-      <c r="A20" s="80" t="s">
+      <c r="A20" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="81" t="str">
+      <c r="B20" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C20" s="81" t="str">
+      <c r="C20" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15">
-      <c r="A21" s="80" t="s">
+      <c r="A21" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="81" t="str">
+      <c r="B21" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C21" s="81" t="str">
+      <c r="C21" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15">
-      <c r="A22" s="80" t="s">
+      <c r="A22" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="81" t="str">
+      <c r="B22" s="78" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C22" s="81" t="str">
+      <c r="C22" s="78" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15">
-      <c r="A23" s="80" t="s">
+      <c r="A23" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="81" t="str">
+      <c r="B23" s="78" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C23" s="81" t="str">
+      <c r="C23" s="78" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15">
-      <c r="A24" s="55" t="s">
+      <c r="A24" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
     </row>
     <row r="25" spans="1:3" ht="15">
-      <c r="A25" s="80" t="s">
+      <c r="A25" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="81" t="str">
+      <c r="B25" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_battery_currents_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
-      <c r="C25" s="81" t="str">
+      <c r="C25" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_battery_currents_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15">
-      <c r="A26" s="80" t="s">
+      <c r="A26" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="81" t="str">
+      <c r="B26" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_alternator_currents_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
-      <c r="C26" s="81" t="str">
+      <c r="C26" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_alternator_currents_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15">
-      <c r="A27" s="80" t="s">
+      <c r="A27" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="81" t="str">
+      <c r="B27" s="78" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
-      <c r="C27" s="81" t="str">
+      <c r="C27" s="78" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15">
-      <c r="A28" s="80" t="s">
+      <c r="A28" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="81" t="str">
+      <c r="B28" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
-      <c r="C28" s="81" t="str">
+      <c r="C28" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15">
-      <c r="A29" s="80" t="s">
+      <c r="A29" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="81" t="str">
+      <c r="B29" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
-      <c r="C29" s="81" t="str">
+      <c r="C29" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15">
-      <c r="A30" s="80" t="s">
+      <c r="A30" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="81" t="str">
+      <c r="B30" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
-      <c r="C30" s="81" t="str">
+      <c r="C30" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15">
-      <c r="A31" s="80" t="s">
+      <c r="A31" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="81" t="str">
+      <c r="B31" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
-      <c r="C31" s="81" t="str">
+      <c r="C31" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15">
-      <c r="A32" s="80" t="s">
+      <c r="A32" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="81" t="str">
+      <c r="B32" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
-      <c r="C32" s="81" t="str">
+      <c r="C32" s="78" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="81" t="str">
+      <c r="B33" s="78" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
-      <c r="C33" s="81" t="str">
+      <c r="C33" s="78" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15">
-      <c r="A34" s="80" t="s">
+      <c r="A34" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="81" t="str">
+      <c r="B34" s="78" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
-      <c r="C34" s="81" t="str">
+      <c r="C34" s="78" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
feat(cold_start), #516: Simplify cold start model, improve thermal, and remove `clutch_tc_speeds`.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C20D0D-4B02-EF4B-93C9-4855479BA645}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2C794C-D0CA-D243-BCB9-E83FE4B2FE86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2231,19 +2231,19 @@
       </c>
       <c r="J17" s="73"/>
       <c r="K17" s="28" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_base_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
       <c r="L17" s="29" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_base_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="M17" s="28" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_base_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
       <c r="N17" s="29" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_base_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="O17" s="18" t="s">

</xml_diff>

<commit_message>
refact(catalyst), #516: Rename cold start model into catalyst model.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2C794C-D0CA-D243-BCB9-E83FE4B2FE86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD847D31-06D7-494D-B0D9-F30C020281D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2231,19 +2231,19 @@
       </c>
       <c r="J17" s="73"/>
       <c r="K17" s="28" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_base_wltp_h_wltp_h_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_catalyst_model_engine_speeds_base_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
       <c r="L17" s="29" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_base_wltp_h_wltp_l_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_catalyst_model_engine_speeds_base_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="M17" s="28" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_base_wltp_l_wltp_h_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_catalyst_model_engine_speeds_base_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
       <c r="N17" s="29" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_base_wltp_l_wltp_l_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_catalyst_model_engine_speeds_base_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="O17" s="18" t="s">

</xml_diff>

<commit_message>
fix(control), #516: Correct catalyst model name.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD847D31-06D7-494D-B0D9-F30C020281D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C31759-170A-114D-91A6-B24C3E604A18}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="82">
   <si>
     <t>Vehicle Family ID</t>
   </si>
@@ -461,6 +461,9 @@
   </si>
   <si>
     <t>electrics_model (dc/dc converter currents)</t>
+  </si>
+  <si>
+    <t>catalyst_speed_model</t>
   </si>
 </sst>
 </file>
@@ -1674,7 +1677,7 @@
   <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
@@ -2227,7 +2230,7 @@
       </c>
       <c r="G17" s="10"/>
       <c r="I17" s="72" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="J17" s="73"/>
       <c r="K17" s="28" t="str">
@@ -3061,7 +3064,6 @@
       <c r="S60" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="D11:E11">
     <cfRule type="colorScale" priority="49">
       <colorScale>

</xml_diff>

<commit_message>
refact(selector), #516: Rename `start_stop_model` to `control_model`.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C31759-170A-114D-91A6-B24C3E604A18}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1F3BA6-1537-0B43-898C-713ADEB7E6D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="84">
   <si>
     <t>Vehicle Family ID</t>
   </si>
@@ -464,6 +464,12 @@
   </si>
   <si>
     <t>catalyst_speed_model</t>
+  </si>
+  <si>
+    <t>control_model (engine starts)</t>
+  </si>
+  <si>
+    <t>control_model (on engine)</t>
   </si>
 </sst>
 </file>
@@ -1677,7 +1683,7 @@
   <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
@@ -2332,7 +2338,7 @@
     <row r="20" spans="2:19" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="G20" s="10"/>
       <c r="I20" s="56" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="J20" s="70"/>
       <c r="K20" s="22" t="str">
@@ -2375,7 +2381,7 @@
       </c>
       <c r="G21" s="10"/>
       <c r="I21" s="62" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="J21" s="71"/>
       <c r="K21" s="37" t="str">
@@ -3064,6 +3070,7 @@
       <c r="S60" s="9"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="D11:E11">
     <cfRule type="colorScale" priority="49">
       <colorScale>

</xml_diff>

<commit_message>
refact(catalyst), #516: Rename `catalyst` --> `after_treatment`.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1F3BA6-1537-0B43-898C-713ADEB7E6D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4F3BB6-7E3E-1D4B-9D4A-B619B1AAFF6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,13 +463,13 @@
     <t>electrics_model (dc/dc converter currents)</t>
   </si>
   <si>
-    <t>catalyst_speed_model</t>
-  </si>
-  <si>
     <t>control_model (engine starts)</t>
   </si>
   <si>
     <t>control_model (on engine)</t>
+  </si>
+  <si>
+    <t>after_treatment_model</t>
   </si>
 </sst>
 </file>
@@ -1683,7 +1683,7 @@
   <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
@@ -2236,23 +2236,23 @@
       </c>
       <c r="G17" s="10"/>
       <c r="I17" s="72" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="J17" s="73"/>
       <c r="K17" s="28" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_catalyst_model_engine_speeds_base_wltp_h_wltp_h_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_after_treatment_model_engine_speeds_base_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
       <c r="L17" s="29" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_catalyst_model_engine_speeds_base_wltp_h_wltp_l_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_after_treatment_model_engine_speeds_base_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="M17" s="28" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_catalyst_model_engine_speeds_base_wltp_l_wltp_h_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_after_treatment_model_engine_speeds_base_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
       <c r="N17" s="29" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_catalyst_model_engine_speeds_base_wltp_l_wltp_l_score"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_after_treatment_model_engine_speeds_base_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="O17" s="18" t="s">
@@ -2338,23 +2338,23 @@
     <row r="20" spans="2:19" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="G20" s="10"/>
       <c r="I20" s="56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J20" s="70"/>
       <c r="K20" s="22" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_h_score"),"")</f>
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_control_model_engine_starts_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
       <c r="L20" s="23" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_l_score"),"")</f>
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_control_model_engine_starts_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="M20" s="22" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_h_score"),"")</f>
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_control_model_engine_starts_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
       <c r="N20" s="23" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_l_score"),"")</f>
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_control_model_engine_starts_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="O20" s="18" t="s">
@@ -2381,23 +2381,23 @@
       </c>
       <c r="G21" s="10"/>
       <c r="I21" s="62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J21" s="71"/>
       <c r="K21" s="37" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_h_score"),"")</f>
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_control_model_on_engine_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
       <c r="L21" s="38" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_l_score"),"")</f>
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_control_model_on_engine_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="M21" s="37" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_h_score"),"")</f>
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_control_model_on_engine_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
       <c r="N21" s="38" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_l_score"),"")</f>
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_control_model_on_engine_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="O21" s="18" t="s">
@@ -3070,7 +3070,6 @@
       <c r="S60" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="D11:E11">
     <cfRule type="colorScale" priority="49">
       <colorScale>

</xml_diff>

<commit_message>
fix(output), #534: Fix report layout.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apps\AIO-TAINTED\CO2MPAS\co2mpas\co2mpas\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4F3BB6-7E3E-1D4B-9D4A-B619B1AAFF6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="16755"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="4" r:id="rId1"/>
     <sheet name="dice_report" sheetId="5" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -475,7 +474,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1435,23 +1434,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1487,23 +1469,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1679,27 +1644,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.1640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="1.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="3" customWidth="1"/>
     <col min="4" max="5" width="12" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.1640625" style="51" customWidth="1"/>
-    <col min="8" max="8" width="1.1640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" style="3" customWidth="1"/>
-    <col min="11" max="14" width="10.6640625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.83203125" style="3" hidden="1"/>
+    <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.140625" style="51" customWidth="1"/>
+    <col min="8" max="8" width="1.140625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" style="3" customWidth="1"/>
+    <col min="11" max="14" width="10.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="3" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" customHeight="1">
@@ -3583,18 +3548,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="34.5" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.5" style="55" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.42578125" style="55" customWidth="1"/>
     <col min="4" max="4" width="8" style="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" style="55" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.83203125" style="55"/>
+    <col min="5" max="5" width="7.42578125" style="55" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.85546875" style="55"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="15">

</xml_diff>

<commit_message>
fix(output), #534: Add dice data to output file.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apps\AIO-TAINTED\CO2MPAS\co2mpas\co2mpas\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FFAE4C-E6F9-3947-B2F6-88121F1B47CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="16755"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="4" r:id="rId1"/>
     <sheet name="dice_report" sheetId="5" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -474,7 +475,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1434,6 +1435,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1469,6 +1487,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1644,27 +1679,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="1.1640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="3" customWidth="1"/>
     <col min="4" max="5" width="12" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.140625" style="51" customWidth="1"/>
-    <col min="8" max="8" width="1.140625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" style="3" customWidth="1"/>
-    <col min="11" max="14" width="10.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="3" hidden="1"/>
+    <col min="6" max="6" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.1640625" style="51" customWidth="1"/>
+    <col min="8" max="8" width="1.1640625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="3" customWidth="1"/>
+    <col min="11" max="14" width="10.6640625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.83203125" style="3" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" customHeight="1">
@@ -1672,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_info_vehicle_family_id_Value"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("dice!_dice_vehicle_family_id_Value"),"")</f>
         <v/>
       </c>
       <c r="E1" s="4"/>
@@ -3548,18 +3583,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.42578125" style="55" customWidth="1"/>
+    <col min="1" max="1" width="34.5" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.5" style="55" customWidth="1"/>
     <col min="4" max="4" width="8" style="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="55" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.85546875" style="55"/>
+    <col min="5" max="5" width="7.5" style="55" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.83203125" style="55"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="15">

</xml_diff>

<commit_message>
feat(report): Add `is_hybrid` to summary report.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FFAE4C-E6F9-3947-B2F6-88121F1B47CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD42503-E515-F643-8F3E-565FDA990056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="output_report" sheetId="4" r:id="rId1"/>
     <sheet name="dice_report" sheetId="5" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="85">
   <si>
     <t>Vehicle Family ID</t>
   </si>
@@ -470,6 +470,9 @@
   </si>
   <si>
     <t>after_treatment_model</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
   </si>
 </sst>
 </file>
@@ -1680,10 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S60"/>
+  <dimension ref="A1:S61"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
@@ -2456,20 +2459,18 @@
     </row>
     <row r="24" spans="2:19" ht="15.75" customHeight="1">
       <c r="B24" s="58" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="C24" s="59"/>
       <c r="D24" s="39" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_is_hybrid__"),"")</f>
         <v/>
       </c>
       <c r="E24" s="40" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__"),"")</f>
-        <v/>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>18</v>
-      </c>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_is_hybrid__"),"")</f>
+        <v/>
+      </c>
+      <c r="F24" s="18"/>
       <c r="G24" s="10"/>
       <c r="I24" s="9"/>
       <c r="P24" s="9"/>
@@ -2477,17 +2478,17 @@
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B25" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="63"/>
-      <c r="D25" s="41" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),"")</f>
-        <v/>
-      </c>
-      <c r="E25" s="42" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__"),"")</f>
+    <row r="25" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B25" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="59"/>
+      <c r="D25" s="39" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),"")</f>
+        <v/>
+      </c>
+      <c r="E25" s="40" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__"),"")</f>
         <v/>
       </c>
       <c r="F25" s="18" t="s">
@@ -2501,10 +2502,21 @@
       <c r="S25" s="9"/>
     </row>
     <row r="26" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="C26" s="35"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="9"/>
+      <c r="B26" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="63"/>
+      <c r="D26" s="41" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),"")</f>
+        <v/>
+      </c>
+      <c r="E26" s="42" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__"),"")</f>
+        <v/>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="G26" s="10"/>
       <c r="I26" s="9"/>
       <c r="P26" s="9"/>
@@ -2513,19 +2525,10 @@
       <c r="S26" s="9"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B27" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>7</v>
-      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="9"/>
       <c r="G27" s="10"/>
       <c r="I27" s="9"/>
       <c r="P27" s="9"/>
@@ -2533,43 +2536,42 @@
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
     </row>
-    <row r="28" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B28" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="20" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_"),"")</f>
-        <v/>
-      </c>
-      <c r="E28" s="21" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f0__N_"),"")</f>
-        <v/>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>38</v>
+    <row r="28" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B28" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="61"/>
+      <c r="D28" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>7</v>
       </c>
       <c r="G28" s="10"/>
+      <c r="I28" s="9"/>
       <c r="P28" s="9"/>
       <c r="Q28" s="9"/>
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
     </row>
     <row r="29" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B29" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="67"/>
-      <c r="D29" s="44" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__"),"")</f>
-        <v/>
-      </c>
-      <c r="E29" s="45" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__"),"")</f>
+      <c r="B29" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="57"/>
+      <c r="D29" s="20" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_"),"")</f>
+        <v/>
+      </c>
+      <c r="E29" s="21" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f0__N_"),"")</f>
         <v/>
       </c>
       <c r="F29" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G29" s="10"/>
       <c r="P29" s="9"/>
@@ -2579,19 +2581,19 @@
     </row>
     <row r="30" spans="2:19" ht="15.75" customHeight="1">
       <c r="B30" s="66" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C30" s="67"/>
       <c r="D30" s="44" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
       <c r="E30" s="45" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
       <c r="F30" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G30" s="10"/>
       <c r="P30" s="9"/>
@@ -2599,21 +2601,21 @@
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
     </row>
-    <row r="31" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="63"/>
-      <c r="D31" s="46" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_"),"")</f>
-        <v/>
-      </c>
-      <c r="E31" s="47" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_mass__kg_"),"")</f>
+    <row r="31" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B31" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="67"/>
+      <c r="D31" s="44" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
+        <v/>
+      </c>
+      <c r="E31" s="45" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
       <c r="F31" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G31" s="10"/>
       <c r="P31" s="9"/>
@@ -2622,11 +2624,21 @@
       <c r="S31" s="9"/>
     </row>
     <row r="32" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="10"/>
+      <c r="B32" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="63"/>
+      <c r="D32" s="46" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_"),"")</f>
+        <v/>
+      </c>
+      <c r="E32" s="47" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_mass__kg_"),"")</f>
+        <v/>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>44</v>
+      </c>
       <c r="G32" s="10"/>
       <c r="P32" s="9"/>
       <c r="Q32" s="9"/>
@@ -2634,40 +2646,30 @@
       <c r="S32" s="9"/>
     </row>
     <row r="33" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B33" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="61"/>
-      <c r="D33" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>7</v>
-      </c>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="9"/>
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
     </row>
-    <row r="34" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B34" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="20" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_"),"")</f>
-        <v/>
-      </c>
-      <c r="E34" s="21" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f0__N_"),"")</f>
-        <v/>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>38</v>
+    <row r="34" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B34" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="61"/>
+      <c r="D34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>7</v>
       </c>
       <c r="G34" s="10"/>
       <c r="P34" s="9"/>
@@ -2676,41 +2678,42 @@
       <c r="S34" s="9"/>
     </row>
     <row r="35" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B35" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="67"/>
-      <c r="D35" s="44" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__"),"")</f>
-        <v/>
-      </c>
-      <c r="E35" s="45" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__"),"")</f>
+      <c r="B35" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="57"/>
+      <c r="D35" s="20" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_"),"")</f>
+        <v/>
+      </c>
+      <c r="E35" s="21" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f0__N_"),"")</f>
         <v/>
       </c>
       <c r="F35" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G35" s="10"/>
+      <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
       <c r="R35" s="9"/>
       <c r="S35" s="9"/>
     </row>
     <row r="36" spans="2:19" ht="15.75" customHeight="1">
       <c r="B36" s="66" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" s="67"/>
       <c r="D36" s="44" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
       <c r="E36" s="45" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
       <c r="F36" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G36" s="10"/>
       <c r="Q36" s="9"/>
@@ -2718,20 +2721,20 @@
       <c r="S36" s="9"/>
     </row>
     <row r="37" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B37" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="59"/>
-      <c r="D37" s="49" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_"),"")</f>
-        <v/>
-      </c>
-      <c r="E37" s="50" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_mass__kg_"),"")</f>
+      <c r="B37" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="67"/>
+      <c r="D37" s="44" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
+        <v/>
+      </c>
+      <c r="E37" s="45" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
       <c r="F37" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G37" s="10"/>
       <c r="Q37" s="9"/>
@@ -2740,19 +2743,19 @@
     </row>
     <row r="38" spans="2:19" ht="15.75" customHeight="1">
       <c r="B38" s="58" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C38" s="59"/>
-      <c r="D38" s="20" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
-        <v/>
-      </c>
-      <c r="E38" s="21" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
+      <c r="D38" s="49" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_"),"")</f>
+        <v/>
+      </c>
+      <c r="E38" s="50" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_mass__kg_"),"")</f>
         <v/>
       </c>
       <c r="F38" s="18" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="G38" s="10"/>
       <c r="Q38" s="9"/>
@@ -2761,15 +2764,15 @@
     </row>
     <row r="39" spans="2:19" ht="15.75" customHeight="1">
       <c r="B39" s="58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="59"/>
       <c r="D39" s="20" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="E39" s="21" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="F39" s="18" t="s">
@@ -2782,15 +2785,15 @@
     </row>
     <row r="40" spans="2:19" ht="15.75" customHeight="1">
       <c r="B40" s="58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" s="59"/>
       <c r="D40" s="20" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="E40" s="21" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="F40" s="18" t="s">
@@ -2801,29 +2804,43 @@
       <c r="R40" s="9"/>
       <c r="S40" s="9"/>
     </row>
-    <row r="41" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B41" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" s="63"/>
-      <c r="D41" s="33" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
-        <v/>
-      </c>
-      <c r="E41" s="34" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
+    <row r="41" spans="2:19" ht="15.75" customHeight="1">
+      <c r="B41" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="59"/>
+      <c r="D41" s="20" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
+        <v/>
+      </c>
+      <c r="E41" s="21" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="F41" s="18" t="s">
         <v>9</v>
       </c>
       <c r="G41" s="10"/>
-      <c r="I41" s="9"/>
       <c r="Q41" s="9"/>
       <c r="R41" s="9"/>
       <c r="S41" s="9"/>
     </row>
-    <row r="42" spans="2:19" ht="15.75" customHeight="1">
+    <row r="42" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B42" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="63"/>
+      <c r="D42" s="33" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
+        <v/>
+      </c>
+      <c r="E42" s="34" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
+        <v/>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="G42" s="10"/>
       <c r="I42" s="9"/>
       <c r="Q42" s="9"/>
@@ -2865,7 +2882,7 @@
       <c r="R47" s="9"/>
       <c r="S47" s="9"/>
     </row>
-    <row r="48" spans="2:19" ht="15.75" hidden="1" customHeight="1">
+    <row r="48" spans="2:19" ht="15.75" customHeight="1">
       <c r="G48" s="10"/>
       <c r="I48" s="9"/>
       <c r="Q48" s="9"/>
@@ -2875,19 +2892,13 @@
     <row r="49" spans="3:19" ht="15.75" hidden="1" customHeight="1">
       <c r="G49" s="10"/>
       <c r="I49" s="9"/>
-      <c r="P49" s="9"/>
       <c r="Q49" s="9"/>
       <c r="R49" s="9"/>
       <c r="S49" s="9"/>
     </row>
-    <row r="50" spans="3:19" ht="15" hidden="1" customHeight="1">
-      <c r="C50" s="6"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="4"/>
+    <row r="50" spans="3:19" ht="15.75" hidden="1" customHeight="1">
+      <c r="G50" s="10"/>
+      <c r="I50" s="9"/>
       <c r="P50" s="9"/>
       <c r="Q50" s="9"/>
       <c r="R50" s="9"/>
@@ -2908,35 +2919,30 @@
     </row>
     <row r="52" spans="3:19" ht="15" hidden="1" customHeight="1">
       <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6"/>
-      <c r="N52" s="6"/>
-      <c r="O52" s="9"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="4"/>
       <c r="P52" s="9"/>
       <c r="Q52" s="9"/>
       <c r="R52" s="9"/>
       <c r="S52" s="9"/>
     </row>
     <row r="53" spans="3:19" ht="15" hidden="1" customHeight="1">
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="10"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-      <c r="K53" s="9"/>
-      <c r="L53" s="9"/>
-      <c r="M53" s="9"/>
-      <c r="N53" s="9"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
       <c r="O53" s="9"/>
       <c r="P53" s="9"/>
       <c r="Q53" s="9"/>
@@ -2944,7 +2950,7 @@
       <c r="S53" s="9"/>
     </row>
     <row r="54" spans="3:19" ht="15" hidden="1" customHeight="1">
-      <c r="C54" s="6"/>
+      <c r="C54" s="9"/>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
@@ -3052,7 +3058,7 @@
       <c r="S59" s="9"/>
     </row>
     <row r="60" spans="3:19" ht="15" hidden="1" customHeight="1">
-      <c r="C60" s="9"/>
+      <c r="C60" s="6"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
@@ -3068,6 +3074,24 @@
       <c r="Q60" s="9"/>
       <c r="R60" s="9"/>
       <c r="S60" s="9"/>
+    </row>
+    <row r="61" spans="3:19" ht="15" hidden="1" customHeight="1">
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="10"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="9"/>
+      <c r="O61" s="9"/>
+      <c r="P61" s="9"/>
+      <c r="Q61" s="9"/>
+      <c r="R61" s="9"/>
+      <c r="S61" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D11:E11">

</xml_diff>

<commit_message>
feat(template): Updated input and output templates.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD42503-E515-F643-8F3E-565FDA990056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2743F6-2CAF-DC47-A868-DC85087C1888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1686,7 +1687,7 @@
   <dimension ref="A1:S61"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
@@ -1892,11 +1893,11 @@
       </c>
       <c r="C9" s="57"/>
       <c r="D9" s="16" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_target_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_target_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_is_plugin_Value"),FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_target_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_is_plugin_Value"),FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="E9" s="17" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_target_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_target_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_is_plugin_Value"),FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_target_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_is_plugin_Value"),FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="F9" s="18" t="s">
@@ -1933,11 +1934,11 @@
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="20" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_is_plugin_Value"),FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_is_plugin_Value"),FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="E10" s="21" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_is_plugin_Value"),FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_is_plugin_Value"),FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="F10" s="18" t="s">
@@ -1978,11 +1979,11 @@
       </c>
       <c r="C11" s="63"/>
       <c r="D11" s="25" t="str">
-        <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100,"")</f>
+        <f ca="1">IFERROR((D10/D9-1)*100,"")</f>
         <v/>
       </c>
       <c r="E11" s="26" t="str">
-        <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio")-1)*100, "")</f>
+        <f ca="1">IFERROR((E10/E9-1)*100,"")</f>
         <v/>
       </c>
       <c r="F11" s="18" t="s">
@@ -2137,11 +2138,11 @@
       </c>
       <c r="C15" s="57"/>
       <c r="D15" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="E15" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_value__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_value__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_value__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="F15" s="18" t="s">
@@ -2182,11 +2183,11 @@
       </c>
       <c r="C16" s="59"/>
       <c r="D16" s="20" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="E16" s="21" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_UDC__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_UDC__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_UDC__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="F16" s="18" t="s">
@@ -2227,11 +2228,11 @@
       </c>
       <c r="C17" s="63"/>
       <c r="D17" s="33" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="E17" s="34" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_EUDC__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_EUDC__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_EUDC__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="F17" s="18" t="s">
@@ -2417,11 +2418,11 @@
       </c>
       <c r="C22" s="57"/>
       <c r="D22" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__"),""))</f>
         <v/>
       </c>
       <c r="E22" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_fuel_type__"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_fuel_type__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_fuel_type__"),""))</f>
         <v/>
       </c>
       <c r="F22" s="18" t="s">
@@ -2440,11 +2441,11 @@
       </c>
       <c r="C23" s="59"/>
       <c r="D23" s="39" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_"),""))</f>
         <v/>
       </c>
       <c r="E23" s="40" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_"),""))</f>
         <v/>
       </c>
       <c r="F23" s="18" t="s">
@@ -2463,11 +2464,11 @@
       </c>
       <c r="C24" s="59"/>
       <c r="D24" s="39" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_is_hybrid__"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_is_hybrid__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_is_hybrid__"),""))</f>
         <v/>
       </c>
       <c r="E24" s="40" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_is_hybrid__"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_is_hybrid__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_is_hybrid__"),""))</f>
         <v/>
       </c>
       <c r="F24" s="18"/>
@@ -2484,11 +2485,11 @@
       </c>
       <c r="C25" s="59"/>
       <c r="D25" s="39" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),""))</f>
         <v/>
       </c>
       <c r="E25" s="40" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__"),""))</f>
         <v/>
       </c>
       <c r="F25" s="18" t="s">
@@ -2507,11 +2508,11 @@
       </c>
       <c r="C26" s="63"/>
       <c r="D26" s="41" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),""))</f>
         <v/>
       </c>
       <c r="E26" s="42" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__"),""))</f>
         <v/>
       </c>
       <c r="F26" s="18" t="s">
@@ -2563,11 +2564,11 @@
       </c>
       <c r="C29" s="57"/>
       <c r="D29" s="20" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_"),""))</f>
         <v/>
       </c>
       <c r="E29" s="21" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f0__N_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f0__N_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f0__N_"),""))</f>
         <v/>
       </c>
       <c r="F29" s="18" t="s">
@@ -2585,11 +2586,11 @@
       </c>
       <c r="C30" s="67"/>
       <c r="D30" s="44" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__"),""))</f>
         <v/>
       </c>
       <c r="E30" s="45" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__"),""))</f>
         <v/>
       </c>
       <c r="F30" s="18" t="s">
@@ -2607,11 +2608,11 @@
       </c>
       <c r="C31" s="67"/>
       <c r="D31" s="44" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_"),""))</f>
         <v/>
       </c>
       <c r="E31" s="45" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_"),""))</f>
         <v/>
       </c>
       <c r="F31" s="18" t="s">
@@ -2629,11 +2630,11 @@
       </c>
       <c r="C32" s="63"/>
       <c r="D32" s="46" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_"),""))</f>
         <v/>
       </c>
       <c r="E32" s="47" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_mass__kg_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_mass__kg_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_mass__kg_"),""))</f>
         <v/>
       </c>
       <c r="F32" s="18" t="s">
@@ -2683,11 +2684,11 @@
       </c>
       <c r="C35" s="57"/>
       <c r="D35" s="20" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_"),""))</f>
         <v/>
       </c>
       <c r="E35" s="21" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f0__N_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f0__N_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f0__N_"),""))</f>
         <v/>
       </c>
       <c r="F35" s="18" t="s">
@@ -2705,11 +2706,11 @@
       </c>
       <c r="C36" s="67"/>
       <c r="D36" s="44" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__"),""))</f>
         <v/>
       </c>
       <c r="E36" s="45" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__"),""))</f>
         <v/>
       </c>
       <c r="F36" s="18" t="s">
@@ -2726,11 +2727,11 @@
       </c>
       <c r="C37" s="67"/>
       <c r="D37" s="44" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_"),""))</f>
         <v/>
       </c>
       <c r="E37" s="45" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_"),""))</f>
         <v/>
       </c>
       <c r="F37" s="18" t="s">
@@ -2747,11 +2748,11 @@
       </c>
       <c r="C38" s="59"/>
       <c r="D38" s="49" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_"),""))</f>
         <v/>
       </c>
       <c r="E38" s="50" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_mass__kg_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_mass__kg_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_mass__kg_"),""))</f>
         <v/>
       </c>
       <c r="F38" s="18" t="s">
@@ -2768,11 +2769,11 @@
       </c>
       <c r="C39" s="59"/>
       <c r="D39" s="20" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="E39" s="21" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="F39" s="18" t="s">
@@ -2789,11 +2790,11 @@
       </c>
       <c r="C40" s="59"/>
       <c r="D40" s="20" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="E40" s="21" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="F40" s="18" t="s">
@@ -2810,11 +2811,11 @@
       </c>
       <c r="C41" s="59"/>
       <c r="D41" s="20" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="E41" s="21" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="F41" s="18" t="s">
@@ -2831,11 +2832,11 @@
       </c>
       <c r="C42" s="63"/>
       <c r="D42" s="33" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="E42" s="34" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="F42" s="18" t="s">

</xml_diff>

<commit_message>
fix(template): Update thermal model limit.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA17C77C-89AA-9440-922F-0B0330AF2240}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F468AE12-BFA7-C045-8B5D-DA921051ADEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1335,7 +1335,21 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3181,7 +3195,7 @@
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="4"/>
         <color rgb="FF00B050"/>
         <color rgb="FFFFC000"/>
       </colorScale>
@@ -3381,7 +3395,7 @@
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="4"/>
         <color rgb="FF00B050"/>
         <color rgb="FFFFC000"/>
       </colorScale>
@@ -3391,7 +3405,7 @@
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="4"/>
         <color rgb="FF00B050"/>
         <color rgb="FFFFC000"/>
       </colorScale>
@@ -3401,7 +3415,7 @@
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="4"/>
         <color rgb="FF00B050"/>
         <color rgb="FFFFC000"/>
       </colorScale>
@@ -3508,10 +3522,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4 J4">
-    <cfRule type="expression" dxfId="1" priority="50">
+    <cfRule type="expression" dxfId="3" priority="50">
       <formula>$C$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="51">
+    <cfRule type="expression" dxfId="2" priority="51">
       <formula>$C$4="True"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix(templates), #567: Correct typo in NEDC-L cell.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F468AE12-BFA7-C045-8B5D-DA921051ADEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDBC504-5484-2F4A-919F-D13FB8F07466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1335,21 +1335,7 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -1911,7 +1897,7 @@
         <v/>
       </c>
       <c r="E9" s="17" t="str">
-        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_target_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_is_plugin_Value"),FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_target_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_is_plugin_Value"),FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),""))</f>
+        <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_l_prediction_target_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_input_type_Value")="OVC-HEV",FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_l_prediction_target_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_input_type_Value")="OVC-HEV",FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),""))</f>
         <v/>
       </c>
       <c r="F9" s="18" t="s">
@@ -3522,10 +3508,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4 J4">
-    <cfRule type="expression" dxfId="3" priority="50">
+    <cfRule type="expression" dxfId="1" priority="50">
       <formula>$C$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="51">
+    <cfRule type="expression" dxfId="0" priority="51">
       <formula>$C$4="True"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix(templates): Remove unused hidden dice report.
</commit_message>
<xml_diff>
--- a/co2mpas/templates/output_template.xlsx
+++ b/co2mpas/templates/output_template.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDBC504-5484-2F4A-919F-D13FB8F07466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E498CC1-B6A8-0942-96B8-4DDCB4D14DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="4" r:id="rId1"/>
-    <sheet name="dice_report" sheetId="5" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="63">
   <si>
     <t>Vehicle Family ID</t>
   </si>
@@ -67,16 +66,10 @@
     <t>WLTP-L</t>
   </si>
   <si>
-    <t>alternator_model (battery currents)</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
     <t>%</t>
-  </si>
-  <si>
-    <t>alternator_model (alternator currents)</t>
   </si>
   <si>
     <t>*Ki factor - corrected</t>
@@ -121,9 +114,6 @@
     </r>
   </si>
   <si>
-    <t>engine_cold_start_speed_model</t>
-  </si>
-  <si>
     <t>engine_coolant_temperature_model</t>
   </si>
   <si>
@@ -133,13 +123,7 @@
     <t>engine_speed_model</t>
   </si>
   <si>
-    <t>start_stop_model (engine starts)</t>
-  </si>
-  <si>
     <t>Vehicle Characteristics</t>
-  </si>
-  <si>
-    <t>start_stop_model (on engine)</t>
   </si>
   <si>
     <t>Parameter</t>
@@ -206,51 +190,6 @@
     <t>Test Mass</t>
   </si>
   <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>vehicle-H</t>
-  </si>
-  <si>
-    <t>vehicle-L</t>
-  </si>
-  <si>
-    <t>vehicle_family_id</t>
-  </si>
-  <si>
-    <t>CO2MPAS_version</t>
-  </si>
-  <si>
-    <t>report_type</t>
-  </si>
-  <si>
-    <t>dice_report</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>TA_mode</t>
-  </si>
-  <si>
-    <t>CO2MPAS_deviation</t>
-  </si>
-  <si>
-    <t>Vehicle</t>
-  </si>
-  <si>
-    <t>fuel_type</t>
-  </si>
-  <si>
-    <t>engine_capacity</t>
-  </si>
-  <si>
-    <t>gear_box_type</t>
-  </si>
-  <si>
-    <t>engine_is_turbo</t>
-  </si>
-  <si>
     <r>
       <t>NEDC Average Specific CO2</t>
     </r>
@@ -444,12 +383,6 @@
       </rPr>
       <t xml:space="preserve"> emission phase Extra-High</t>
     </r>
-  </si>
-  <si>
-    <t>Model_scores WLTP-H</t>
-  </si>
-  <si>
-    <t>Model_scores WLTP-L</t>
   </si>
   <si>
     <t>electrics_model (service battery currents)</t>
@@ -1005,7 +938,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1211,22 +1144,6 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
@@ -1308,14 +1225,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="7"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1687,7 +1596,7 @@
   <dimension ref="A1:S61"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
@@ -1829,24 +1738,24 @@
       <c r="S5" s="9"/>
     </row>
     <row r="6" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
+        <v>45</v>
+      </c>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
       <c r="G6" s="12"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
       <c r="K6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
@@ -1860,10 +1769,10 @@
       <c r="S7" s="9"/>
     </row>
     <row r="8" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B8" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="61"/>
+      <c r="B8" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="57"/>
       <c r="D8" s="13" t="s">
         <v>5</v>
       </c>
@@ -1874,24 +1783,24 @@
         <v>7</v>
       </c>
       <c r="G8" s="10"/>
-      <c r="K8" s="76" t="s">
+      <c r="K8" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="75"/>
-      <c r="M8" s="76" t="s">
+      <c r="L8" s="71"/>
+      <c r="M8" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="75"/>
+      <c r="N8" s="71"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
     </row>
     <row r="9" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B9" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="57"/>
+      <c r="B9" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="53"/>
       <c r="D9" s="16" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_target_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_input_type_Value")="OVC-HEV",FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_target_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_input_type_Value")="OVC-HEV",FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),""))</f>
         <v/>
@@ -1904,10 +1813,10 @@
         <v>9</v>
       </c>
       <c r="G9" s="10"/>
-      <c r="I9" s="68" t="s">
+      <c r="I9" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="69"/>
+      <c r="J9" s="65"/>
       <c r="K9" s="19" t="s">
         <v>10</v>
       </c>
@@ -1920,7 +1829,7 @@
       <c r="N9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="74" t="s">
+      <c r="O9" s="70" t="s">
         <v>7</v>
       </c>
       <c r="P9" s="9"/>
@@ -1929,10 +1838,10 @@
       <c r="S9" s="9"/>
     </row>
     <row r="10" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B10" s="58" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="59"/>
+      <c r="B10" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="55"/>
       <c r="D10" s="20" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_input_type_Value")="OVC-HEV",FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_declared"&amp;IF(IFERROR(INDIRECT("dice!_dice_input_type_Value")="OVC-HEV",FALSE), "_sustaining","")&amp;"_co2_emission_value__CO2g_km_"),""))</f>
         <v/>
@@ -1945,10 +1854,10 @@
         <v>9</v>
       </c>
       <c r="G10" s="10"/>
-      <c r="I10" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="J10" s="70"/>
+      <c r="I10" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="66"/>
       <c r="K10" s="22" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_service_battery_currents_wltp_h_wltp_h_score"),"")</f>
         <v/>
@@ -1966,7 +1875,7 @@
         <v/>
       </c>
       <c r="O10" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
@@ -1974,10 +1883,10 @@
       <c r="S10" s="9"/>
     </row>
     <row r="11" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B11" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="63"/>
+      <c r="B11" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="59"/>
       <c r="D11" s="25" t="str">
         <f ca="1">IFERROR((D10/D9-1)*100,"")</f>
         <v/>
@@ -1987,31 +1896,31 @@
         <v/>
       </c>
       <c r="F11" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="10"/>
-      <c r="I11" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="J11" s="79"/>
-      <c r="K11" s="80" t="str">
+      <c r="I11" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="73"/>
+      <c r="K11" s="74" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_alternator_currents_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="L11" s="81" t="str">
+      <c r="L11" s="75" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_alternator_currents_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
-      <c r="M11" s="80" t="str">
+      <c r="M11" s="74" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_alternator_currents_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="N11" s="81" t="str">
+      <c r="N11" s="75" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_alternator_currents_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="O11" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
@@ -2019,36 +1928,36 @@
       <c r="S11" s="9"/>
     </row>
     <row r="12" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B12" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="64"/>
+      <c r="B12" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="60"/>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
       <c r="F12" s="9"/>
       <c r="G12" s="10"/>
-      <c r="I12" s="58" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" s="79"/>
-      <c r="K12" s="80" t="str">
+      <c r="I12" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="73"/>
+      <c r="K12" s="74" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_drive_battery_currents_wltp_h_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="L12" s="81" t="str">
+      <c r="L12" s="75" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_drive_battery_currents_wltp_h_wltp_l_score"),"")</f>
         <v/>
       </c>
-      <c r="M12" s="80" t="str">
+      <c r="M12" s="74" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_drive_battery_currents_wltp_l_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="N12" s="81" t="str">
+      <c r="N12" s="75" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_drive_battery_currents_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="O12" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
@@ -2061,10 +1970,10 @@
       <c r="E13" s="30"/>
       <c r="F13" s="9"/>
       <c r="G13" s="10"/>
-      <c r="I13" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="J13" s="71"/>
+      <c r="I13" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="67"/>
       <c r="K13" s="37" t="str">
         <f ca="1">IF(K12&lt;&gt;"",IFERROR(INDIRECT("data.calibration.model_scores!_scores_electrics_model_dcdc_converter_currents_wltp_h_wltp_h_score"),""),"")</f>
         <v/>
@@ -2082,7 +1991,7 @@
         <v/>
       </c>
       <c r="O13" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
@@ -2090,10 +1999,10 @@
       <c r="S13" s="9"/>
     </row>
     <row r="14" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B14" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="61"/>
+      <c r="B14" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="57"/>
       <c r="D14" s="13" t="s">
         <v>5</v>
       </c>
@@ -2104,10 +2013,10 @@
         <v>7</v>
       </c>
       <c r="G14" s="10"/>
-      <c r="I14" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="73"/>
+      <c r="I14" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="69"/>
       <c r="K14" s="28" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_h_wltp_h_score"),"")</f>
         <v/>
@@ -2125,7 +2034,7 @@
         <v/>
       </c>
       <c r="O14" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
@@ -2133,10 +2042,10 @@
       <c r="S14" s="9"/>
     </row>
     <row r="15" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B15" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="57"/>
+      <c r="B15" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="53"/>
       <c r="D15" s="31" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_"),""))</f>
         <v/>
@@ -2149,10 +2058,10 @@
         <v>9</v>
       </c>
       <c r="G15" s="10"/>
-      <c r="I15" s="72" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="73"/>
+      <c r="I15" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="69"/>
       <c r="K15" s="28" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
         <v/>
@@ -2170,7 +2079,7 @@
         <v/>
       </c>
       <c r="O15" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
@@ -2178,10 +2087,10 @@
       <c r="S15" s="9"/>
     </row>
     <row r="16" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B16" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="59"/>
+      <c r="B16" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="55"/>
       <c r="D16" s="20" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_"),""))</f>
         <v/>
@@ -2194,10 +2103,10 @@
         <v>9</v>
       </c>
       <c r="G16" s="10"/>
-      <c r="I16" s="72" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="73"/>
+      <c r="I16" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="69"/>
       <c r="K16" s="28" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_h_wltp_h_score"),"")</f>
         <v/>
@@ -2215,7 +2124,7 @@
         <v/>
       </c>
       <c r="O16" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
@@ -2223,10 +2132,10 @@
       <c r="S16" s="9"/>
     </row>
     <row r="17" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B17" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="63"/>
+      <c r="B17" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="59"/>
       <c r="D17" s="33" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_"),""))</f>
         <v/>
@@ -2239,10 +2148,10 @@
         <v>9</v>
       </c>
       <c r="G17" s="10"/>
-      <c r="I17" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="J17" s="73"/>
+      <c r="I17" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="69"/>
       <c r="K17" s="28" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_after_treatment_model_engine_speeds_base_wltp_h_wltp_h_score"),"")</f>
         <v/>
@@ -2260,7 +2169,7 @@
         <v/>
       </c>
       <c r="O17" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
@@ -2273,10 +2182,10 @@
       <c r="E18" s="36"/>
       <c r="F18" s="9"/>
       <c r="G18" s="10"/>
-      <c r="I18" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18" s="73"/>
+      <c r="I18" s="68" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="69"/>
       <c r="K18" s="28" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_h_score"),"")</f>
         <v/>
@@ -2294,7 +2203,7 @@
         <v/>
       </c>
       <c r="O18" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
@@ -2302,19 +2211,19 @@
       <c r="S18" s="9"/>
     </row>
     <row r="19" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
+        <v>24</v>
+      </c>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
       <c r="G19" s="12"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="72" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="73"/>
+      <c r="I19" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="69"/>
       <c r="K19" s="28" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
         <v/>
@@ -2332,7 +2241,7 @@
         <v/>
       </c>
       <c r="O19" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="9"/>
@@ -2341,10 +2250,10 @@
     </row>
     <row r="20" spans="2:19" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="G20" s="10"/>
-      <c r="I20" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="J20" s="70"/>
+      <c r="I20" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="66"/>
       <c r="K20" s="22" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_control_model_engine_starts_wltp_h_wltp_h_score"),"")</f>
         <v/>
@@ -2362,7 +2271,7 @@
         <v/>
       </c>
       <c r="O20" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
@@ -2370,10 +2279,10 @@
       <c r="S20" s="9"/>
     </row>
     <row r="21" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B21" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="61"/>
+      <c r="B21" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="57"/>
       <c r="D21" s="13" t="s">
         <v>5</v>
       </c>
@@ -2384,10 +2293,10 @@
         <v>7</v>
       </c>
       <c r="G21" s="10"/>
-      <c r="I21" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="J21" s="71"/>
+      <c r="I21" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21" s="67"/>
       <c r="K21" s="37" t="str">
         <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_control_model_on_engine_wltp_h_wltp_h_score"),"")</f>
         <v/>
@@ -2405,7 +2314,7 @@
         <v/>
       </c>
       <c r="O21" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
@@ -2413,10 +2322,10 @@
       <c r="S21" s="9"/>
     </row>
     <row r="22" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B22" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="57"/>
+      <c r="B22" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="53"/>
       <c r="D22" s="31" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__"),""))</f>
         <v/>
@@ -2426,7 +2335,7 @@
         <v/>
       </c>
       <c r="F22" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G22" s="10"/>
       <c r="I22" s="9"/>
@@ -2436,10 +2345,10 @@
       <c r="S22" s="9"/>
     </row>
     <row r="23" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B23" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="59"/>
+      <c r="B23" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="55"/>
       <c r="D23" s="39" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_"),""))</f>
         <v/>
@@ -2449,7 +2358,7 @@
         <v/>
       </c>
       <c r="F23" s="18" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G23" s="10"/>
       <c r="I23" s="9"/>
@@ -2459,10 +2368,10 @@
       <c r="S23" s="9"/>
     </row>
     <row r="24" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B24" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="59"/>
+      <c r="B24" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="55"/>
       <c r="D24" s="39" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_is_hybrid__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_is_hybrid__"),""))</f>
         <v/>
@@ -2480,10 +2389,10 @@
       <c r="S24" s="9"/>
     </row>
     <row r="25" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B25" s="58" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="59"/>
+      <c r="B25" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="55"/>
       <c r="D25" s="39" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),""))</f>
         <v/>
@@ -2493,7 +2402,7 @@
         <v/>
       </c>
       <c r="F25" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G25" s="10"/>
       <c r="I25" s="9"/>
@@ -2503,10 +2412,10 @@
       <c r="S25" s="9"/>
     </row>
     <row r="26" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B26" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="63"/>
+      <c r="B26" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="59"/>
       <c r="D26" s="41" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),""))</f>
         <v/>
@@ -2516,7 +2425,7 @@
         <v/>
       </c>
       <c r="F26" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G26" s="10"/>
       <c r="I26" s="9"/>
@@ -2538,10 +2447,10 @@
       <c r="S27" s="9"/>
     </row>
     <row r="28" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B28" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="61"/>
+      <c r="B28" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="57"/>
       <c r="D28" s="13" t="s">
         <v>5</v>
       </c>
@@ -2559,10 +2468,10 @@
       <c r="S28" s="9"/>
     </row>
     <row r="29" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B29" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="57"/>
+      <c r="B29" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="53"/>
       <c r="D29" s="20" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_"),""))</f>
         <v/>
@@ -2572,7 +2481,7 @@
         <v/>
       </c>
       <c r="F29" s="18" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G29" s="10"/>
       <c r="P29" s="9"/>
@@ -2581,10 +2490,10 @@
       <c r="S29" s="9"/>
     </row>
     <row r="30" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B30" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="67"/>
+      <c r="B30" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="63"/>
       <c r="D30" s="44" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__"),""))</f>
         <v/>
@@ -2594,7 +2503,7 @@
         <v/>
       </c>
       <c r="F30" s="18" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G30" s="10"/>
       <c r="P30" s="9"/>
@@ -2603,10 +2512,10 @@
       <c r="S30" s="9"/>
     </row>
     <row r="31" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B31" s="66" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="67"/>
+      <c r="B31" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="63"/>
       <c r="D31" s="44" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_"),""))</f>
         <v/>
@@ -2616,7 +2525,7 @@
         <v/>
       </c>
       <c r="F31" s="18" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G31" s="10"/>
       <c r="P31" s="9"/>
@@ -2625,10 +2534,10 @@
       <c r="S31" s="9"/>
     </row>
     <row r="32" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B32" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="63"/>
+      <c r="B32" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="59"/>
       <c r="D32" s="46" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_"),"")="","",IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_"),""))</f>
         <v/>
@@ -2638,7 +2547,7 @@
         <v/>
       </c>
       <c r="F32" s="18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G32" s="10"/>
       <c r="P32" s="9"/>
@@ -2659,10 +2568,10 @@
       <c r="S33" s="9"/>
     </row>
     <row r="34" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B34" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="61"/>
+      <c r="B34" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="57"/>
       <c r="D34" s="13" t="s">
         <v>5</v>
       </c>
@@ -2679,10 +2588,10 @@
       <c r="S34" s="9"/>
     </row>
     <row r="35" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B35" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="57"/>
+      <c r="B35" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="53"/>
       <c r="D35" s="20" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_"),""))</f>
         <v/>
@@ -2692,7 +2601,7 @@
         <v/>
       </c>
       <c r="F35" s="18" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G35" s="10"/>
       <c r="P35" s="9"/>
@@ -2701,10 +2610,10 @@
       <c r="S35" s="9"/>
     </row>
     <row r="36" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B36" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="67"/>
+      <c r="B36" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="63"/>
       <c r="D36" s="44" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__"),""))</f>
         <v/>
@@ -2714,7 +2623,7 @@
         <v/>
       </c>
       <c r="F36" s="18" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G36" s="10"/>
       <c r="Q36" s="9"/>
@@ -2722,10 +2631,10 @@
       <c r="S36" s="9"/>
     </row>
     <row r="37" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B37" s="66" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="67"/>
+      <c r="B37" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="63"/>
       <c r="D37" s="44" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_"),""))</f>
         <v/>
@@ -2735,7 +2644,7 @@
         <v/>
       </c>
       <c r="F37" s="18" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G37" s="10"/>
       <c r="Q37" s="9"/>
@@ -2743,10 +2652,10 @@
       <c r="S37" s="9"/>
     </row>
     <row r="38" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B38" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="59"/>
+      <c r="B38" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="55"/>
       <c r="D38" s="49" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_"),""))</f>
         <v/>
@@ -2756,7 +2665,7 @@
         <v/>
       </c>
       <c r="F38" s="18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G38" s="10"/>
       <c r="Q38" s="9"/>
@@ -2764,10 +2673,10 @@
       <c r="S38" s="9"/>
     </row>
     <row r="39" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B39" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="59"/>
+      <c r="B39" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="55"/>
       <c r="D39" s="20" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_"),""))</f>
         <v/>
@@ -2785,10 +2694,10 @@
       <c r="S39" s="9"/>
     </row>
     <row r="40" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B40" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="59"/>
+      <c r="B40" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="55"/>
       <c r="D40" s="20" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_"),""))</f>
         <v/>
@@ -2806,10 +2715,10 @@
       <c r="S40" s="9"/>
     </row>
     <row r="41" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B41" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="59"/>
+      <c r="B41" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="55"/>
       <c r="D41" s="20" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_"),""))</f>
         <v/>
@@ -2827,10 +2736,10 @@
       <c r="S41" s="9"/>
     </row>
     <row r="42" spans="2:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B42" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="63"/>
+      <c r="B42" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="59"/>
       <c r="D42" s="33" t="str">
         <f ca="1">IF(IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_"),"")="","",IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_"),""))</f>
         <v/>
@@ -3605,451 +3514,4 @@
     <brk id="6" max="1048575" man="1"/>
   </colBreaks>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C34"/>
-  <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="12"/>
-  <cols>
-    <col min="1" max="1" width="34.5" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.5" style="55" customWidth="1"/>
-    <col min="4" max="4" width="8" style="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" style="55" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.83203125" style="55"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A1" s="52" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="52" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="2" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_info_vehicle_family_id_Value"),"")</f>
-        <v/>
-      </c>
-      <c r="C2" s="2" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_info_vehicle_family_id_Value"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_info_CO2MPAS_version_Value"),"")</f>
-        <v/>
-      </c>
-      <c r="C3" s="2" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_info_CO2MPAS_version_Value"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="2" t="str">
-        <f>B4</f>
-        <v>dice_report</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="2" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_info_Simulation_started_Value"),"")</f>
-        <v/>
-      </c>
-      <c r="C5" s="2" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_info_Simulation_started_Value"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_info_type_approval_mode_Value"),"")</f>
-        <v/>
-      </c>
-      <c r="C6" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_info_type_approval_mode_Value"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A7" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="53" t="str">
-        <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100,"")</f>
-        <v/>
-      </c>
-      <c r="C7" s="53" t="str">
-        <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio")-1)*100,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A8" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-    </row>
-    <row r="9" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A9" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="39" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__"),"")</f>
-        <v/>
-      </c>
-      <c r="C9" s="39" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_fuel_type__"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A10" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="39" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
-        <v/>
-      </c>
-      <c r="C10" s="39" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A11" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="39" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),"")</f>
-        <v/>
-      </c>
-      <c r="C11" s="39" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="3" customFormat="1" ht="15">
-      <c r="A12" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="39" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),"")</f>
-        <v/>
-      </c>
-      <c r="C12" s="39" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15">
-      <c r="A13" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-    </row>
-    <row r="14" spans="1:3" ht="15">
-      <c r="A14" s="77" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_battery_currents_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C14" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_battery_currents_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15">
-      <c r="A15" s="77" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_alternator_currents_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C15" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_alternator_currents_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15">
-      <c r="A16" s="77" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="78" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C16" s="78" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15">
-      <c r="A17" s="77" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C17" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15">
-      <c r="A18" s="77" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C18" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15">
-      <c r="A19" s="77" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C19" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15">
-      <c r="A20" s="77" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C20" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15">
-      <c r="A21" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C21" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15">
-      <c r="A22" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="78" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C22" s="78" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15">
-      <c r="A23" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="78" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C23" s="78" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15">
-      <c r="A24" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-    </row>
-    <row r="25" spans="1:3" ht="15">
-      <c r="A25" s="77" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_battery_currents_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C25" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_battery_currents_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15">
-      <c r="A26" s="77" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_alternator_currents_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C26" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_alternator_model_alternator_currents_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15">
-      <c r="A27" s="77" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="78" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C27" s="78" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_at_model_gears_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15">
-      <c r="A28" s="77" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C28" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_clutch_torque_converter_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15">
-      <c r="A29" s="77" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C29" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_co2_params_identified_co2_emissions_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15">
-      <c r="A30" s="77" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C30" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_cold_start_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15">
-      <c r="A31" s="77" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C31" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15">
-      <c r="A32" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C32" s="78" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15">
-      <c r="A33" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="78" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C33" s="78" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15">
-      <c r="A34" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="78" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C34" s="78" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Bold"CO&amp;Y2&amp;YMPAS DICE REPORT</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>